<commit_message>
Minor correction to BOM
</commit_message>
<xml_diff>
--- a/Resources/BOM.xlsx
+++ b/Resources/BOM.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <fileSharing readOnlyRecommended="0" userName="micro"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rocky\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0302CBC9-8B34-4DA6-B774-84B7E113C92D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcOnSave="0"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="smNativeData">
       <pm:revision xmlns:pm="smNativeData" day="1605153511" val="978" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
       <pm:docPrefs xmlns:pm="smNativeData" id="1605153511" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
@@ -77,9 +91,6 @@
   </si>
   <si>
     <t>ALZ11B05W-ND</t>
-  </si>
-  <si>
-    <t>MID-SIZE SPST OFF-ON BULB DC</t>
   </si>
   <si>
     <t>SW2</t>
@@ -465,83 +476,36 @@
   <si>
     <t>Does not include enclosure or launch battery.</t>
   </si>
+  <si>
+    <t>SWITCH ROCKER SPST 16A 125V</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="5" formatCode="#,##0\ &quot;$&quot;;\-#,##0\ &quot;$&quot;"/>
-    <numFmt numFmtId="6" formatCode="#,##0\ &quot;$&quot;;[Red]\-#,##0\ &quot;$&quot;"/>
-    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;$&quot;;\-#,##0.00\ &quot;$&quot;"/>
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;;[Red]\-#,##0.00\ &quot;$&quot;"/>
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;$&quot;_-;\-* #,##0\ &quot;$&quot;_-;_-* &quot;-&quot;\ &quot;$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="[$$-409]0.00_);([$$-409]0.00)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="[$$-409]0.00_);\([$$-409]0.00\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605153511" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Times New Roman" sz="200" lang="default"/>
-            <pm:ea face="SimSun" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
     <font>
-      <name val="Basic Sans"/>
-      <family val="1"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605153511" ulstyle="none" kern="1">
-            <pm:latin face="Basic Sans" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605153511" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default"/>
-            <pm:cs face="Basic Roman" sz="200" lang="default"/>
-            <pm:ea face="Basic Roman" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <b/>
-      <color rgb="FF000000"/>
-      <sz val="10"/>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1605153511" ulstyle="none" kern="1">
-            <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
-            <pm:cs face="Times New Roman" sz="200" lang="default"/>
-            <pm:ea face="SimSun" sz="200" lang="default"/>
-          </pm:charSpec>
-        </ext>
-      </extLst>
     </font>
   </fonts>
   <fills count="4">
@@ -555,120 +519,81 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB5B5B5"/>
         <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1605153511" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
-          </ext>
-        </extLst>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1605153511" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
       </patternFill>
     </fill>
   </fills>
   <borders count="3">
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1605153511"/>
-        </ext>
-      </extLst>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1605153511"/>
-        </ext>
-      </extLst>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1605153511"/>
-        </ext>
-      </extLst>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
     <ext uri="smNativeData">
       <pm:charStyles xmlns:pm="smNativeData" id="1605153511" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
@@ -687,10 +612,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="D5D5D5"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="494949"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="EEECE1"/>
@@ -937,30 +862,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="70" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
+  <sheetFormatPr defaultColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.621622" customWidth="1" style="1"/>
-    <col min="2" max="2" width="27.567568" customWidth="1" style="1"/>
-    <col min="3" max="3" width="42.972973" customWidth="1" style="1"/>
-    <col min="4" max="4" width="42.567568" customWidth="1" style="1"/>
-    <col min="5" max="5" width="29.324324" customWidth="1" style="1"/>
-    <col min="6" max="6" width="10.819820" customWidth="1" style="1"/>
-    <col min="7" max="7" width="33.243243" customWidth="1" style="1"/>
-    <col min="8" max="8" width="10.000000" style="1"/>
-    <col min="9" max="9" width="11.081081" customWidth="1" style="1"/>
-    <col min="10" max="10" width="10.270270" customWidth="1" style="1"/>
-    <col min="11" max="11" width="72.333333" customWidth="1" style="1"/>
-    <col min="12" max="16383" width="10.000000" style="1"/>
+    <col min="1" max="1" width="36.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43" style="1" customWidth="1"/>
+    <col min="4" max="4" width="42.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10" style="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="72.28515625" style="1" customWidth="1"/>
+    <col min="12" max="16383" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16384" s="3" customFormat="1">
+    <row r="1" spans="1:16384" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -17368,7 +17293,7 @@
       <c r="XFC1" s="4"/>
       <c r="XFD1" s="4"/>
     </row>
-    <row r="2" spans="1:16384">
+    <row r="2" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -17390,654 +17315,654 @@
       <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>1</v>
       </c>
-      <c r="I2" s="2" t="n">
-        <v>2.83000000000000007</v>
-      </c>
-      <c r="J2" s="2" t="n">
-        <v>2.83000000000000007</v>
+      <c r="I2" s="2">
+        <v>2.83</v>
+      </c>
+      <c r="J2" s="2">
+        <v>2.83</v>
       </c>
       <c r="XFD2" s="1"/>
     </row>
-    <row r="3" spans="1:16384">
+    <row r="3" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="H3" s="1">
         <v>1</v>
       </c>
-      <c r="I3" s="2" t="n">
-        <v>1.06000000000000005</v>
-      </c>
-      <c r="J3" s="2" t="n">
-        <v>1.06000000000000005</v>
+      <c r="I3" s="2">
+        <v>1.06</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.06</v>
       </c>
       <c r="XFD3" s="1"/>
     </row>
-    <row r="4" spans="1:16384">
+    <row r="4" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="n">
-        <v>0.569999999999999929</v>
-      </c>
-      <c r="J4" s="2" t="n">
-        <v>0.569999999999999929</v>
+      <c r="I4" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.56999999999999995</v>
       </c>
       <c r="XFD4" s="1"/>
     </row>
-    <row r="5" spans="1:16384">
+    <row r="5" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="H5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="2" t="n">
-        <v>2.60999999999999988</v>
-      </c>
-      <c r="J5" s="2" t="n">
-        <v>2.60999999999999988</v>
+      <c r="I5" s="2">
+        <v>2.61</v>
+      </c>
+      <c r="J5" s="2">
+        <v>2.61</v>
       </c>
       <c r="XFD5" s="1"/>
     </row>
-    <row r="6" spans="1:16384">
+    <row r="6" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="H6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="2" t="n">
-        <v>0.210000000000000009</v>
-      </c>
-      <c r="J6" s="2" t="n">
-        <v>0.210000000000000009</v>
+      <c r="I6" s="2">
+        <v>0.21000000000000002</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.21000000000000002</v>
       </c>
       <c r="XFD6" s="1"/>
     </row>
-    <row r="7" spans="1:16384">
+    <row r="7" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H7" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="H7" s="1">
         <v>1</v>
       </c>
-      <c r="I7" s="2" t="n">
-        <v>1.66999999999999993</v>
-      </c>
-      <c r="J7" s="2" t="n">
-        <v>1.66999999999999993</v>
+      <c r="I7" s="2">
+        <v>1.67</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1.67</v>
       </c>
       <c r="XFD7" s="1"/>
     </row>
-    <row r="8" spans="1:16384">
+    <row r="8" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="H8" s="1">
         <v>1</v>
       </c>
-      <c r="I8" s="2" t="n">
+      <c r="I8" s="2">
         <v>0.2</v>
       </c>
-      <c r="J8" s="2" t="n">
+      <c r="J8" s="2">
         <v>0.2</v>
       </c>
       <c r="XFD8" s="1"/>
     </row>
-    <row r="9" spans="1:16384">
+    <row r="9" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="H9" s="1">
         <v>2</v>
       </c>
-      <c r="I9" s="2" t="n">
+      <c r="I9" s="2">
         <v>0.1</v>
       </c>
-      <c r="J9" s="2" t="n">
+      <c r="J9" s="2">
         <v>0.2</v>
       </c>
       <c r="XFD9" s="1"/>
     </row>
-    <row r="10" spans="1:16384">
+    <row r="10" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="H10" s="1">
         <v>2</v>
       </c>
-      <c r="I10" s="2" t="n">
+      <c r="I10" s="2">
         <v>0.1</v>
       </c>
-      <c r="J10" s="2" t="n">
+      <c r="J10" s="2">
         <v>0.2</v>
       </c>
       <c r="XFD10" s="1"/>
     </row>
-    <row r="11" spans="1:16384">
+    <row r="11" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="H11" s="1">
         <v>2</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I11" s="2">
         <v>0.1</v>
       </c>
-      <c r="J11" s="2" t="n">
+      <c r="J11" s="2">
         <v>0.2</v>
       </c>
       <c r="XFD11" s="1"/>
     </row>
-    <row r="12" spans="1:16384">
+    <row r="12" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="n">
+      <c r="I12" s="2">
         <v>0.1</v>
       </c>
-      <c r="J12" s="2" t="n">
+      <c r="J12" s="2">
         <v>0.1</v>
       </c>
       <c r="XFD12" s="1"/>
     </row>
-    <row r="13" spans="1:16384">
+    <row r="13" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H13" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="H13" s="1">
         <v>1</v>
       </c>
-      <c r="I13" s="2" t="n">
+      <c r="I13" s="2">
         <v>0.1</v>
       </c>
-      <c r="J13" s="2" t="n">
+      <c r="J13" s="2">
         <v>0.1</v>
       </c>
       <c r="XFD13" s="1"/>
     </row>
-    <row r="14" spans="1:16384">
+    <row r="14" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="H14" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="H14" s="1">
         <v>2</v>
       </c>
-      <c r="I14" s="2" t="n">
+      <c r="I14" s="2">
         <v>0.1</v>
       </c>
-      <c r="J14" s="2" t="n">
+      <c r="J14" s="2">
         <v>0.2</v>
       </c>
       <c r="XFD14" s="1"/>
     </row>
-    <row r="15" spans="1:16384">
+    <row r="15" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H15" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="H15" s="1">
         <v>2</v>
       </c>
-      <c r="I15" s="2" t="n">
+      <c r="I15" s="2">
         <v>0.1</v>
       </c>
-      <c r="J15" s="2" t="n">
+      <c r="J15" s="2">
         <v>0.2</v>
       </c>
       <c r="XFD15" s="1"/>
     </row>
-    <row r="16" spans="1:16384">
+    <row r="16" spans="1:16384" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="E16" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>91</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H16" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="H16" s="1">
         <v>1</v>
       </c>
-      <c r="I16" s="2" t="n">
-        <v>0.230000000000000027</v>
-      </c>
-      <c r="J16" s="2" t="n">
-        <v>0.230000000000000027</v>
+      <c r="I16" s="2">
+        <v>0.23000000000000004</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.23000000000000004</v>
       </c>
       <c r="XFD16" s="1"/>
     </row>
-    <row r="17" spans="1:16384">
+    <row r="17" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="E17" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="H17" s="1">
         <v>1</v>
       </c>
-      <c r="I17" s="2" t="n">
+      <c r="I17" s="2">
         <v>0.65</v>
       </c>
-      <c r="J17" s="2" t="n">
+      <c r="J17" s="2">
         <v>0.65</v>
       </c>
       <c r="XFD17" s="1"/>
     </row>
-    <row r="18" spans="1:16384">
+    <row r="18" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="D18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="I18" s="2">
+        <v>0.59</v>
+      </c>
+      <c r="J18" s="2">
+        <v>1.18</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="I18" s="2" t="n">
-        <v>0.589999999999999947</v>
-      </c>
-      <c r="J18" s="2" t="n">
-        <v>1.17999999999999994</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>106</v>
       </c>
       <c r="XFD18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="15.70" customHeight="1">
+    <row r="19" spans="1:11 16384:16384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="I19" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="J19" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I19" s="2" t="n">
-        <v>2.56999999999999984</v>
-      </c>
-      <c r="J19" s="2" t="n">
-        <v>2.56999999999999984</v>
-      </c>
-      <c r="K19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="5" t="s">
+      <c r="B20" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>117</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>118</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="6" t="n">
-        <v>5.95000000000000018</v>
-      </c>
-      <c r="J20" s="6" t="n">
-        <v>5.95000000000000018</v>
+        <v>112</v>
+      </c>
+      <c r="I20" s="6">
+        <v>5.95</v>
+      </c>
+      <c r="J20" s="6">
+        <v>5.95</v>
       </c>
       <c r="K20" s="5"/>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>122</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>123</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" s="6">
+        <v>2.08</v>
+      </c>
+      <c r="J21" s="6">
+        <v>4.16</v>
+      </c>
+      <c r="K21" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="H21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I21" s="6" t="n">
-        <v>2.08000000000000007</v>
-      </c>
-      <c r="J21" s="6" t="n">
-        <v>4.16000000000000014</v>
-      </c>
-      <c r="K21" s="5" t="s">
+    </row>
+    <row r="22" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -18050,142 +17975,127 @@
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
-    <row r="23" spans="1:16384">
+    <row r="23" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="C23" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="E23" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" s="5" t="s">
+      <c r="G23" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="7">
+        <v>4.66</v>
+      </c>
+      <c r="J23" s="7">
+        <v>13.99</v>
+      </c>
+      <c r="K23" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="I23" s="7" t="n">
-        <v>4.66000000000000014</v>
-      </c>
-      <c r="J23" s="7" t="n">
-        <v>13.9900000000000002</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="XFD23" s="1"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="B24" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="D24" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="H24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.37</v>
+      </c>
+      <c r="J24" s="8">
+        <v>8.99</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="I24" s="8" t="n">
-        <v>0.370000000000000018</v>
-      </c>
-      <c r="J24" s="8" t="n">
-        <v>8.99000000000000021</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>139</v>
+      <c r="G25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I25" s="8">
+        <v>4.99</v>
+      </c>
+      <c r="J25" s="8">
+        <v>9.99</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="I25" s="8" t="n">
-        <v>4.99000000000000021</v>
-      </c>
-      <c r="J25" s="8" t="n">
-        <v>9.99000000000000021</v>
-      </c>
-      <c r="K25" s="1" t="s">
+    <row r="26" spans="1:11 16384:16384" x14ac:dyDescent="0.2">
+      <c r="I26" s="9" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="9:11">
-      <c r="I26" s="9" t="s">
-        <v>145</v>
       </c>
       <c r="J26" s="9">
         <f>SUM(J2:J25)</f>
-        <v>58.0600000000000023</v>
+        <v>58.06</v>
       </c>
       <c r="K26" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
-  <printOptions>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1605153511" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
-      </ext>
-    </extLst>
-  </printOptions>
-  <pageMargins left="0.787500" right="0.787500" top="0.787500" bottom="0.787500" header="0.393750" footer="0.393750"/>
-  <pageSetup paperSize="1" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown"/>
-  <headerFooter>
-    <extLst>
-      <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1605153511" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1605153511" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-      </ext>
-    </extLst>
-  </headerFooter>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.78749999999999998" bottom="0.78749999999999998" header="0.39374999999999999" footer="0.39374999999999999"/>
+  <pageSetup fitToWidth="0" pageOrder="overThenDown"/>
   <extLst>
     <ext uri="smNativeData">
       <pm:sheetPrefs xmlns:pm="smNativeData" day="1605153511" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">

</xml_diff>